<commit_message>
train and test data prep
</commit_message>
<xml_diff>
--- a/Data/Defense_2014.csv.xlsx
+++ b/Data/Defense_2014.csv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kobe/Desktop/FinTech/TouchdownProphet/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Desktop\Project_3\TouchdownProphet\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8657FE5-9F85-4F45-AB10-C515764369FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{55AFF334-C458-4798-BE69-73477815E14E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{EC768BE9-C832-4A67-ACD7-5E75AFE0B3A4}"/>
+    <workbookView xWindow="-22428" yWindow="612" windowWidth="21600" windowHeight="11292" xr2:uid="{EC768BE9-C832-4A67-ACD7-5E75AFE0B3A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -111,6 +111,12 @@
     <t>First Downs by Penalty</t>
   </si>
   <si>
+    <t>% of Drives Ending in Offensive Score Allowed</t>
+  </si>
+  <si>
+    <t>% of Drives Ending in Takeaways</t>
+  </si>
+  <si>
     <t>Expected Points Contributed by All Defense</t>
   </si>
   <si>
@@ -217,12 +223,6 @@
   </si>
   <si>
     <t>Avg Tm/G</t>
-  </si>
-  <si>
-    <t>% of Drives Ending in Offensive Score Allowed</t>
-  </si>
-  <si>
-    <t>% of Drives Ending in Takeaways</t>
   </si>
 </sst>
 </file>
@@ -576,42 +576,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9951300E-D4B8-484D-A36E-E1C38F9BD16C}">
   <dimension ref="A1:AB36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:AB36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="34.1640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -688,21 +659,21 @@
         <v>24</v>
       </c>
       <c r="Z1" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="AA1" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="AB1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <v>16</v>
@@ -783,12 +754,12 @@
         <v>40.92</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C3">
         <v>16</v>
@@ -869,12 +840,12 @@
         <v>-16.38</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C4">
         <v>16</v>
@@ -955,12 +926,12 @@
         <v>53.86</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C5">
         <v>16</v>
@@ -1041,12 +1012,12 @@
         <v>43.28</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C6">
         <v>16</v>
@@ -1127,12 +1098,12 @@
         <v>-9.75</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C7">
         <v>16</v>
@@ -1213,12 +1184,12 @@
         <v>-18.91</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C8">
         <v>16</v>
@@ -1299,12 +1270,12 @@
         <v>75.87</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C9">
         <v>16</v>
@@ -1385,12 +1356,12 @@
         <v>-51.58</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C10">
         <v>16</v>
@@ -1471,12 +1442,12 @@
         <v>-11.69</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C11">
         <v>16</v>
@@ -1557,12 +1528,12 @@
         <v>-11.11</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C12">
         <v>16</v>
@@ -1643,12 +1614,12 @@
         <v>-39.67</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C13">
         <v>16</v>
@@ -1729,12 +1700,12 @@
         <v>-39.01</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C14">
         <v>16</v>
@@ -1815,12 +1786,12 @@
         <v>-52.29</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C15">
         <v>16</v>
@@ -1901,12 +1872,12 @@
         <v>-33.950000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C16">
         <v>16</v>
@@ -1987,12 +1958,12 @@
         <v>-69.98</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C17">
         <v>16</v>
@@ -2073,12 +2044,12 @@
         <v>5.24</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C18">
         <v>16</v>
@@ -2159,12 +2130,12 @@
         <v>3.47</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C19">
         <v>16</v>
@@ -2245,12 +2216,12 @@
         <v>-73.84</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C20">
         <v>16</v>
@@ -2331,12 +2302,12 @@
         <v>-12</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C21">
         <v>16</v>
@@ -2417,12 +2388,12 @@
         <v>-28.48</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C22">
         <v>16</v>
@@ -2503,12 +2474,12 @@
         <v>-38.36</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C23">
         <v>16</v>
@@ -2589,12 +2560,12 @@
         <v>-31.44</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C24">
         <v>16</v>
@@ -2675,12 +2646,12 @@
         <v>-58.87</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C25">
         <v>16</v>
@@ -2761,12 +2732,12 @@
         <v>-70.400000000000006</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C26">
         <v>16</v>
@@ -2847,12 +2818,12 @@
         <v>-84.36</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C27">
         <v>16</v>
@@ -2933,12 +2904,12 @@
         <v>-46.95</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C28">
         <v>16</v>
@@ -3019,12 +2990,12 @@
         <v>-128.96</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C29">
         <v>16</v>
@@ -3105,12 +3076,12 @@
         <v>-128.38</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C30">
         <v>16</v>
@@ -3191,12 +3162,12 @@
         <v>-121.72</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C31">
         <v>16</v>
@@ -3277,12 +3248,12 @@
         <v>-111.18</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C32">
         <v>16</v>
@@ -3363,12 +3334,12 @@
         <v>-102.23</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C33">
         <v>16</v>
@@ -3449,9 +3420,9 @@
         <v>-57.69</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D34">
         <v>361.4</v>
@@ -3529,9 +3500,9 @@
         <v>-38.299999999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D35">
         <v>11565</v>
@@ -3606,9 +3577,9 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D36">
         <v>22.6</v>

</xml_diff>

<commit_message>
train and test sets completed
</commit_message>
<xml_diff>
--- a/Data/Defense_2014.csv.xlsx
+++ b/Data/Defense_2014.csv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Desktop\Project_3\TouchdownProphet\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kobe/Desktop/TouchdownProphet/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55AFF334-C458-4798-BE69-73477815E14E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4F51B5-9108-4349-AAD4-032CA48F5239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22428" yWindow="612" windowWidth="21600" windowHeight="11292" xr2:uid="{EC768BE9-C832-4A67-ACD7-5E75AFE0B3A4}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{EC768BE9-C832-4A67-ACD7-5E75AFE0B3A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -111,12 +111,6 @@
     <t>First Downs by Penalty</t>
   </si>
   <si>
-    <t>% of Drives Ending in Offensive Score Allowed</t>
-  </si>
-  <si>
-    <t>% of Drives Ending in Takeaways</t>
-  </si>
-  <si>
     <t>Expected Points Contributed by All Defense</t>
   </si>
   <si>
@@ -223,6 +217,12 @@
   </si>
   <si>
     <t>Avg Tm/G</t>
+  </si>
+  <si>
+    <t>% Drives Ending in Offensive Score Allowed</t>
+  </si>
+  <si>
+    <t>% Drives Ending in Takeaways</t>
   </si>
 </sst>
 </file>
@@ -577,12 +577,12 @@
   <dimension ref="A1:AB36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:AB36"/>
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -659,21 +659,21 @@
         <v>24</v>
       </c>
       <c r="Z1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>27</v>
-      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2">
         <v>16</v>
@@ -754,12 +754,12 @@
         <v>40.92</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>16</v>
@@ -840,12 +840,12 @@
         <v>-16.38</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>16</v>
@@ -926,12 +926,12 @@
         <v>53.86</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>16</v>
@@ -1012,12 +1012,12 @@
         <v>43.28</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>16</v>
@@ -1098,12 +1098,12 @@
         <v>-9.75</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7">
         <v>16</v>
@@ -1184,12 +1184,12 @@
         <v>-18.91</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8">
         <v>16</v>
@@ -1270,12 +1270,12 @@
         <v>75.87</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C9">
         <v>16</v>
@@ -1356,12 +1356,12 @@
         <v>-51.58</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C10">
         <v>16</v>
@@ -1442,12 +1442,12 @@
         <v>-11.69</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C11">
         <v>16</v>
@@ -1528,12 +1528,12 @@
         <v>-11.11</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C12">
         <v>16</v>
@@ -1614,12 +1614,12 @@
         <v>-39.67</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C13">
         <v>16</v>
@@ -1700,12 +1700,12 @@
         <v>-39.01</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C14">
         <v>16</v>
@@ -1786,12 +1786,12 @@
         <v>-52.29</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15">
         <v>16</v>
@@ -1872,12 +1872,12 @@
         <v>-33.950000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C16">
         <v>16</v>
@@ -1958,12 +1958,12 @@
         <v>-69.98</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C17">
         <v>16</v>
@@ -2044,12 +2044,12 @@
         <v>5.24</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18">
         <v>16</v>
@@ -2130,12 +2130,12 @@
         <v>3.47</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C19">
         <v>16</v>
@@ -2216,12 +2216,12 @@
         <v>-73.84</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C20">
         <v>16</v>
@@ -2302,12 +2302,12 @@
         <v>-12</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C21">
         <v>16</v>
@@ -2388,12 +2388,12 @@
         <v>-28.48</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C22">
         <v>16</v>
@@ -2474,12 +2474,12 @@
         <v>-38.36</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C23">
         <v>16</v>
@@ -2560,12 +2560,12 @@
         <v>-31.44</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C24">
         <v>16</v>
@@ -2646,12 +2646,12 @@
         <v>-58.87</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C25">
         <v>16</v>
@@ -2732,12 +2732,12 @@
         <v>-70.400000000000006</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C26">
         <v>16</v>
@@ -2818,12 +2818,12 @@
         <v>-84.36</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C27">
         <v>16</v>
@@ -2904,12 +2904,12 @@
         <v>-46.95</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C28">
         <v>16</v>
@@ -2990,12 +2990,12 @@
         <v>-128.96</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C29">
         <v>16</v>
@@ -3076,12 +3076,12 @@
         <v>-128.38</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C30">
         <v>16</v>
@@ -3162,12 +3162,12 @@
         <v>-121.72</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C31">
         <v>16</v>
@@ -3248,12 +3248,12 @@
         <v>-111.18</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C32">
         <v>16</v>
@@ -3334,12 +3334,12 @@
         <v>-102.23</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C33">
         <v>16</v>
@@ -3420,9 +3420,9 @@
         <v>-57.69</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D34">
         <v>361.4</v>
@@ -3500,9 +3500,9 @@
         <v>-38.299999999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D35">
         <v>11565</v>
@@ -3577,9 +3577,9 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D36">
         <v>22.6</v>

</xml_diff>

<commit_message>
xgboost and lr added
</commit_message>
<xml_diff>
--- a/Data/Defense_2014.csv.xlsx
+++ b/Data/Defense_2014.csv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kobe/Desktop/TouchdownProphet/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Desktop\Project_3\TouchdownProphet\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4F51B5-9108-4349-AAD4-032CA48F5239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{55AFF334-C458-4798-BE69-73477815E14E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{EC768BE9-C832-4A67-ACD7-5E75AFE0B3A4}"/>
+    <workbookView xWindow="-22428" yWindow="612" windowWidth="21600" windowHeight="11292" xr2:uid="{EC768BE9-C832-4A67-ACD7-5E75AFE0B3A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -111,6 +111,12 @@
     <t>First Downs by Penalty</t>
   </si>
   <si>
+    <t>% of Drives Ending in Offensive Score Allowed</t>
+  </si>
+  <si>
+    <t>% of Drives Ending in Takeaways</t>
+  </si>
+  <si>
     <t>Expected Points Contributed by All Defense</t>
   </si>
   <si>
@@ -217,12 +223,6 @@
   </si>
   <si>
     <t>Avg Tm/G</t>
-  </si>
-  <si>
-    <t>% Drives Ending in Offensive Score Allowed</t>
-  </si>
-  <si>
-    <t>% Drives Ending in Takeaways</t>
   </si>
 </sst>
 </file>
@@ -577,12 +577,12 @@
   <dimension ref="A1:AB36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1"/>
+      <selection activeCell="A2" sqref="A2:AB36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -659,21 +659,21 @@
         <v>24</v>
       </c>
       <c r="Z1" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="AA1" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="AB1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <v>16</v>
@@ -754,12 +754,12 @@
         <v>40.92</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C3">
         <v>16</v>
@@ -840,12 +840,12 @@
         <v>-16.38</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C4">
         <v>16</v>
@@ -926,12 +926,12 @@
         <v>53.86</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C5">
         <v>16</v>
@@ -1012,12 +1012,12 @@
         <v>43.28</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C6">
         <v>16</v>
@@ -1098,12 +1098,12 @@
         <v>-9.75</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C7">
         <v>16</v>
@@ -1184,12 +1184,12 @@
         <v>-18.91</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C8">
         <v>16</v>
@@ -1270,12 +1270,12 @@
         <v>75.87</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C9">
         <v>16</v>
@@ -1356,12 +1356,12 @@
         <v>-51.58</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C10">
         <v>16</v>
@@ -1442,12 +1442,12 @@
         <v>-11.69</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C11">
         <v>16</v>
@@ -1528,12 +1528,12 @@
         <v>-11.11</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C12">
         <v>16</v>
@@ -1614,12 +1614,12 @@
         <v>-39.67</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C13">
         <v>16</v>
@@ -1700,12 +1700,12 @@
         <v>-39.01</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C14">
         <v>16</v>
@@ -1786,12 +1786,12 @@
         <v>-52.29</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C15">
         <v>16</v>
@@ -1872,12 +1872,12 @@
         <v>-33.950000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C16">
         <v>16</v>
@@ -1958,12 +1958,12 @@
         <v>-69.98</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C17">
         <v>16</v>
@@ -2044,12 +2044,12 @@
         <v>5.24</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C18">
         <v>16</v>
@@ -2130,12 +2130,12 @@
         <v>3.47</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C19">
         <v>16</v>
@@ -2216,12 +2216,12 @@
         <v>-73.84</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C20">
         <v>16</v>
@@ -2302,12 +2302,12 @@
         <v>-12</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C21">
         <v>16</v>
@@ -2388,12 +2388,12 @@
         <v>-28.48</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C22">
         <v>16</v>
@@ -2474,12 +2474,12 @@
         <v>-38.36</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C23">
         <v>16</v>
@@ -2560,12 +2560,12 @@
         <v>-31.44</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C24">
         <v>16</v>
@@ -2646,12 +2646,12 @@
         <v>-58.87</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C25">
         <v>16</v>
@@ -2732,12 +2732,12 @@
         <v>-70.400000000000006</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C26">
         <v>16</v>
@@ -2818,12 +2818,12 @@
         <v>-84.36</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C27">
         <v>16</v>
@@ -2904,12 +2904,12 @@
         <v>-46.95</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C28">
         <v>16</v>
@@ -2990,12 +2990,12 @@
         <v>-128.96</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C29">
         <v>16</v>
@@ -3076,12 +3076,12 @@
         <v>-128.38</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C30">
         <v>16</v>
@@ -3162,12 +3162,12 @@
         <v>-121.72</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C31">
         <v>16</v>
@@ -3248,12 +3248,12 @@
         <v>-111.18</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C32">
         <v>16</v>
@@ -3334,12 +3334,12 @@
         <v>-102.23</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C33">
         <v>16</v>
@@ -3420,9 +3420,9 @@
         <v>-57.69</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D34">
         <v>361.4</v>
@@ -3500,9 +3500,9 @@
         <v>-38.299999999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D35">
         <v>11565</v>
@@ -3577,9 +3577,9 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D36">
         <v>22.6</v>

</xml_diff>